<commit_message>
Update data and cheklist
commonName auth : S1#111ENGINNERING
subject_application_vendor : Engineering Ingegneria Informatica S.p.A
subject_application_id : Ellipse AMB
subject_application_version : 4.0.0
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_AMB/4.0.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_AMB/4.0.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit-my.sharepoint.com/personal/cristiano_avella_eng_it/Documents/Documenti/GitHub/it-fse-accreditamento/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_AMB/4.0.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user597\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="13_ncr:1_{5C6FC6EA-0309-4679-ACAA-4EB3CA69E50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B92ED977-0DB5-4F8E-8A61-20D5F67B4D79}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20992AAD-6726-4FCE-B679-BD9636BA1A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4166,15 +4166,6 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.b514abebdf85aa90f67bcd48d75b0397c6cffb298c1618a8a6f48512ba4b349a.ea35e53b9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>1bccd6f8fb7e3caf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.54ec540407742d72de3ba2bb9388978501ef2da6741cd89927c5f891d9cc3a50.dcc7fa0648^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-29T17:31:33.54Z</t>
-  </si>
-  <si>
     <t>Ellipse AMB</t>
   </si>
   <si>
@@ -4241,28 +4232,37 @@
 Da backoffice sarà possibile per l'operatore in un secondo momento andare a correggere l'errore individuato e a rieseguire con l'eventuale supporto del presidio Engineering il processo di validazione del referto di ambulatorio.</t>
   </si>
   <si>
-    <t>2024-03-04T17:10:10.01Z</t>
-  </si>
-  <si>
-    <t>81725c384ae645ab</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.d5b10cdcb342af42fee7bf2f3382f561c281a5f8a23d435efa007777735b0d40.891e308747^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-03-04T17:26:02.65Z</t>
-  </si>
-  <si>
-    <t>003003b3491c5755</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.ad3a480e21999817480242f4cf24dd62fd3ad87f2c53b6486be5175021e85efc.d4f47bd575^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Test non eseguibile. L'applicativo non gestisce alcune delle informazioni opzionali relative alle prestazioni richieste nel CT tra cui Procedure, SubstanceAdministration, Observation e Act della Procedura Operativa Eseguita.</t>
   </si>
   <si>
     <t>4.0.0</t>
+  </si>
+  <si>
+    <t>2024-03-21T12:50:39.98Z</t>
+  </si>
+  <si>
+    <t>4db8e65faa31d9de</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.38cc66a99026c4ddeedd0750ea8e804304f476894e2045dbff0d5a4499db5f51.83e4a40f6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-21T15:21:50.63Z</t>
+  </si>
+  <si>
+    <t>e6ca4004c83b14ba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.b2c21726143145765d672a3a5d361bc874d17383e078d9f0a7fdbfe542d45311.f48da2798f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-21T15:38:45.19Z</t>
+  </si>
+  <si>
+    <t>faeae0768e5d1f44</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.2026c1b5fc29dfe356562a231955f8581dc460c4caaca37ba1f59702d492ff77.204213c2a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7169,11 +7169,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H39" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I163" sqref="I163"/>
+      <selection pane="bottomRight" activeCell="F157" sqref="F157:I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7243,7 +7243,7 @@
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="45" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="D3" s="37"/>
       <c r="F3" s="12"/>
@@ -7266,7 +7266,7 @@
       <c r="A4" s="41"/>
       <c r="B4" s="42"/>
       <c r="C4" s="45" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="4"/>
@@ -7290,7 +7290,7 @@
       <c r="A5" s="43"/>
       <c r="B5" s="44"/>
       <c r="C5" s="45" t="s">
-        <v>907</v>
+        <v>898</v>
       </c>
       <c r="D5" s="37"/>
       <c r="F5" s="12"/>
@@ -8453,13 +8453,13 @@
         <v>114</v>
       </c>
       <c r="N39" s="25" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="O39" s="25" t="s">
         <v>115</v>
       </c>
       <c r="P39" s="25" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -8745,13 +8745,13 @@
         <v>114</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>115</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -9037,7 +9037,7 @@
         <v>115</v>
       </c>
       <c r="P55" s="25" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -12447,16 +12447,16 @@
         <v>332</v>
       </c>
       <c r="F155" s="23">
-        <v>45351</v>
+        <v>45372</v>
       </c>
       <c r="G155" s="24" t="s">
-        <v>886</v>
+        <v>899</v>
       </c>
       <c r="H155" s="24" t="s">
-        <v>884</v>
+        <v>900</v>
       </c>
       <c r="I155" s="24" t="s">
-        <v>885</v>
+        <v>901</v>
       </c>
       <c r="J155" s="25" t="s">
         <v>114</v>
@@ -12491,16 +12491,16 @@
         <v>334</v>
       </c>
       <c r="F156" s="23">
-        <v>45355</v>
+        <v>45372</v>
       </c>
       <c r="G156" s="24" t="s">
+        <v>902</v>
+      </c>
+      <c r="H156" s="24" t="s">
         <v>903</v>
       </c>
-      <c r="H156" s="24" t="s">
+      <c r="I156" s="24" t="s">
         <v>904</v>
-      </c>
-      <c r="I156" s="24" t="s">
-        <v>905</v>
       </c>
       <c r="J156" s="25" t="s">
         <v>114</v>
@@ -12535,16 +12535,16 @@
         <v>336</v>
       </c>
       <c r="F157" s="23">
-        <v>45355</v>
+        <v>45372</v>
       </c>
       <c r="G157" s="24" t="s">
-        <v>900</v>
+        <v>905</v>
       </c>
       <c r="H157" s="24" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="I157" s="24" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="J157" s="25" t="s">
         <v>114</v>
@@ -12607,7 +12607,7 @@
         <v>114</v>
       </c>
       <c r="P158" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="Q158" s="25"/>
       <c r="R158" s="26"/>
@@ -12698,7 +12698,7 @@
         <v>115</v>
       </c>
       <c r="P160" s="25" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Q160" s="25"/>
       <c r="R160" s="26"/>
@@ -12827,7 +12827,7 @@
         <v>114</v>
       </c>
       <c r="P163" s="25" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
@@ -12919,7 +12919,7 @@
         <v>114</v>
       </c>
       <c r="P165" s="25" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="Q165" s="25"/>
       <c r="R165" s="26"/>
@@ -13011,7 +13011,7 @@
         <v>114</v>
       </c>
       <c r="P167" s="25" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -13120,7 +13120,7 @@
         <v>115</v>
       </c>
       <c r="K170" s="25" t="s">
-        <v>906</v>
+        <v>897</v>
       </c>
       <c r="L170" s="25"/>
       <c r="M170" s="25"/>
@@ -13331,7 +13331,7 @@
         <v>114</v>
       </c>
       <c r="P175" s="25" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="Q175" s="25"/>
       <c r="R175" s="26"/>
@@ -13385,7 +13385,7 @@
         <v>114</v>
       </c>
       <c r="P176" s="25" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="Q176" s="25"/>
       <c r="R176" s="26"/>
@@ -27864,15 +27864,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B4FBF822A1A2C840B5F363470C32238D" ma:contentTypeVersion="14" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="280af7476cdb634aa23cde6f54c24f0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aef395d-7620-4f80-b867-2c9a442e0fc6" xmlns:ns3="c1840d89-b9fd-4af1-bd26-22dfd625d914" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01f0ce4f7644a7368c037f965ce10eaa" ns2:_="" ns3:_="">
     <xsd:import namespace="2aef395d-7620-4f80-b867-2c9a442e0fc6"/>
@@ -28101,15 +28092,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC851931-A0E2-4F9B-9D8E-0633CAD6294D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1840d89-b9fd-4af1-bd26-22dfd625d914">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2aef395d-7620-4f80-b867-2c9a442e0fc6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82AF9BC4-7FCC-4469-90DE-B5E7E59E1C6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28126,4 +28129,16 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC851931-A0E2-4F9B-9D8E-0633CAD6294D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D25B490F-4F2E-41B3-A90A-A3DE0760B01E}"/>
 </file>
</xml_diff>

<commit_message>
Update PDF and files data and cheklist
commonName auth : S1#111ENGINNERING
subject_application_vendor : Engineering Ingegneria Informatica S.p.A
subject_application_id : Ellipse AMB
subject_application_version : 4.0.0
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_AMB/4.0.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_AMB/4.0.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user597\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user597\Desktop\Eng\Call per test FSE\Nuovo giro di test 25.03\File_aggiornati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20992AAD-6726-4FCE-B679-BD9636BA1A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998723F0-8857-4FA8-B680-729A585362A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4238,31 +4238,31 @@
     <t>4.0.0</t>
   </si>
   <si>
-    <t>2024-03-21T12:50:39.98Z</t>
-  </si>
-  <si>
-    <t>4db8e65faa31d9de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.38cc66a99026c4ddeedd0750ea8e804304f476894e2045dbff0d5a4499db5f51.83e4a40f6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-03-21T15:21:50.63Z</t>
-  </si>
-  <si>
-    <t>e6ca4004c83b14ba</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.b2c21726143145765d672a3a5d361bc874d17383e078d9f0a7fdbfe542d45311.f48da2798f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-03-21T15:38:45.19Z</t>
-  </si>
-  <si>
-    <t>faeae0768e5d1f44</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.2026c1b5fc29dfe356562a231955f8581dc460c4caaca37ba1f59702d492ff77.204213c2a4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>37cb5e9eedef097f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.514218bec0d06777fc23cdecb4db7f2d1cc96c06a6d0c11ed5a2c66673125e40.880a1ef245^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-25T15:59:30.88Z</t>
+  </si>
+  <si>
+    <t>215dae7d40345f39</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.cd549151859029b95314a171ea7f5db09c9a8e39848bad6fbb9c6ef7ce8fdd37.7e0c0c41f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-25T16:40:43.15Z</t>
+  </si>
+  <si>
+    <t>917aff572d6e9ad8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.4e8ef5a30b0ba90de0206e3d74a57b9931e3aaa23dd9718015652e9205ac93a7.ac6676c586^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-25T17:04:05.76Z</t>
   </si>
 </sst>
 </file>
@@ -7170,10 +7170,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F157" sqref="F157:I157"/>
+      <selection pane="bottomRight" activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7366,7 +7366,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="40.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20">
         <v>32</v>
       </c>
@@ -8706,7 +8706,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="20">
         <v>40</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="20">
         <v>48</v>
       </c>
@@ -12386,7 +12386,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="20">
         <v>147</v>
       </c>
@@ -12430,7 +12430,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="20">
         <v>148</v>
       </c>
@@ -12447,16 +12447,16 @@
         <v>332</v>
       </c>
       <c r="F155" s="23">
-        <v>45372</v>
+        <v>45376</v>
       </c>
       <c r="G155" s="24" t="s">
+        <v>901</v>
+      </c>
+      <c r="H155" s="24" t="s">
         <v>899</v>
       </c>
-      <c r="H155" s="24" t="s">
+      <c r="I155" s="24" t="s">
         <v>900</v>
-      </c>
-      <c r="I155" s="24" t="s">
-        <v>901</v>
       </c>
       <c r="J155" s="25" t="s">
         <v>114</v>
@@ -12474,7 +12474,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="20">
         <v>149</v>
       </c>
@@ -12491,16 +12491,16 @@
         <v>334</v>
       </c>
       <c r="F156" s="23">
-        <v>45372</v>
+        <v>45376</v>
       </c>
       <c r="G156" s="24" t="s">
+        <v>904</v>
+      </c>
+      <c r="H156" s="24" t="s">
         <v>902</v>
       </c>
-      <c r="H156" s="24" t="s">
+      <c r="I156" s="24" t="s">
         <v>903</v>
-      </c>
-      <c r="I156" s="24" t="s">
-        <v>904</v>
       </c>
       <c r="J156" s="25" t="s">
         <v>114</v>
@@ -12518,7 +12518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="20">
         <v>150</v>
       </c>
@@ -12535,16 +12535,16 @@
         <v>336</v>
       </c>
       <c r="F157" s="23">
-        <v>45372</v>
+        <v>45376</v>
       </c>
       <c r="G157" s="24" t="s">
+        <v>907</v>
+      </c>
+      <c r="H157" s="24" t="s">
         <v>905</v>
       </c>
-      <c r="H157" s="24" t="s">
+      <c r="I157" s="24" t="s">
         <v>906</v>
-      </c>
-      <c r="I157" s="24" t="s">
-        <v>907</v>
       </c>
       <c r="J157" s="25" t="s">
         <v>114</v>
@@ -12562,7 +12562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="20">
         <v>151</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="20">
         <v>152</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A160" s="20">
         <v>153</v>
       </c>
@@ -12707,7 +12707,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="20">
         <v>154</v>
       </c>
@@ -12744,7 +12744,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A162" s="20">
         <v>155</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A163" s="20">
         <v>156</v>
       </c>
@@ -12836,7 +12836,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="20">
         <v>157</v>
       </c>
@@ -12874,7 +12874,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A165" s="20">
         <v>158</v>
       </c>
@@ -12928,7 +12928,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="20">
         <v>159</v>
       </c>
@@ -12966,7 +12966,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="20">
         <v>160</v>
       </c>
@@ -13020,7 +13020,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A168" s="20">
         <v>161</v>
       </c>
@@ -27864,6 +27864,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B4FBF822A1A2C840B5F363470C32238D" ma:contentTypeVersion="14" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="280af7476cdb634aa23cde6f54c24f0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2aef395d-7620-4f80-b867-2c9a442e0fc6" xmlns:ns3="c1840d89-b9fd-4af1-bd26-22dfd625d914" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01f0ce4f7644a7368c037f965ce10eaa" ns2:_="" ns3:_="">
     <xsd:import namespace="2aef395d-7620-4f80-b867-2c9a442e0fc6"/>
@@ -28092,15 +28101,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -28113,6 +28113,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC851931-A0E2-4F9B-9D8E-0633CAD6294D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82AF9BC4-7FCC-4469-90DE-B5E7E59E1C6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28131,14 +28139,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC851931-A0E2-4F9B-9D8E-0633CAD6294D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D25B490F-4F2E-41B3-A90A-A3DE0760B01E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A84B16B3-FF07-472E-8A9F-E5B51293B9D4}"/>
 </file>
</xml_diff>